<commit_message>
change checklists, verifying Multiop
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\TKVM\FLOATING-POINTING_ALU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dai_hoc\LSILogicDesign\FLOATING-POINTING_ALU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DBDB8A-32D6-48C9-B51E-084F6A266677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046CC6E-B135-48CE-B425-0780E1DE10F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="13" r:id="rId1"/>
@@ -57,15 +57,15 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
+    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
     <customWorkbookView name="Giang Truong Le. Nguyen - Personal View" guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
-    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
-    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>&lt;Revision history&gt;</t>
   </si>
@@ -142,31 +142,37 @@
     <t>Version 01, 03/20/2024</t>
   </si>
   <si>
-    <t>Function Check</t>
-  </si>
-  <si>
     <t>Bound Flasher</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>addOp check</t>
   </si>
   <si>
-    <t>testbench and simulation</t>
+    <t>Check addition operator between 2 positive parameters</t>
   </si>
   <si>
-    <t>addOp_check</t>
+    <t>addOp check in normal cases</t>
   </si>
   <si>
-    <t>subOp_check1</t>
+    <t>Check addition operator between a positive parameter and a negative one</t>
   </si>
   <si>
-    <t>subOp_check2</t>
+    <t>Check addition operator between 2 negative parameters</t>
   </si>
   <si>
-    <t>Check subtraction operation of 2 32-bit input para1 and para2 when para1 &gt; para2</t>
+    <t>addOp check in overflow cases</t>
   </si>
   <si>
-    <t>Check addition operation of 2 32-bit input para1 and para2</t>
+    <t>addOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>addOp check in special cases</t>
+  </si>
+  <si>
+    <t>Add a number with zero</t>
+  </si>
+  <si>
+    <t>Add a number with its multiplicative inverse value</t>
   </si>
 </sst>
 </file>
@@ -5174,10 +5180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:AS15"/>
+  <dimension ref="B2:AS19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="15"/>
@@ -5311,7 +5317,7 @@
       </c>
       <c r="C7" s="77"/>
       <c r="D7" s="78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="51"/>
@@ -5379,143 +5385,191 @@
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="47">
         <v>1</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="47">
         <v>1</v>
       </c>
       <c r="G10" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="45" t="s">
-        <v>28</v>
-      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:45" ht="30">
       <c r="B11" s="42"/>
       <c r="C11" s="46"/>
-      <c r="D11" s="47">
-        <v>2</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>30</v>
-      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="47">
         <v>2</v>
       </c>
       <c r="G11" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="45" t="s">
-        <v>28</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="59"/>
     </row>
     <row r="12" spans="2:45" ht="30">
       <c r="B12" s="42"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="47">
-        <v>3</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="47">
         <v>3</v>
       </c>
       <c r="G12" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="45"/>
       <c r="L12" s="60"/>
     </row>
-    <row r="13" spans="2:45" ht="15.6">
+    <row r="13" spans="2:45" ht="30">
       <c r="B13" s="42"/>
       <c r="C13" s="29"/>
       <c r="D13" s="47">
-        <v>4</v>
-      </c>
-      <c r="E13" s="48"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>31</v>
+      </c>
       <c r="F13" s="47">
-        <v>4</v>
-      </c>
-      <c r="G13" s="55"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
       <c r="K13" s="45"/>
       <c r="L13" s="60"/>
     </row>
-    <row r="14" spans="2:45" ht="16.2" thickBot="1">
+    <row r="14" spans="2:45" ht="30">
       <c r="B14" s="42"/>
       <c r="C14" s="29"/>
       <c r="D14" s="47">
-        <v>5</v>
-      </c>
-      <c r="E14" s="48"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="47">
-        <v>5</v>
-      </c>
-      <c r="G14" s="55"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>30</v>
+      </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
       <c r="K14" s="45"/>
-      <c r="L14" s="44"/>
+      <c r="L14" s="60"/>
     </row>
-    <row r="15" spans="2:45" ht="16.8" thickTop="1" thickBot="1">
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="27"/>
+    <row r="15" spans="2:45" ht="15.6">
+      <c r="B15" s="42"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="47">
+        <v>4</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="47">
+        <v>1</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="60"/>
+    </row>
+    <row r="16" spans="2:45" ht="15.6">
+      <c r="B16" s="42"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="47">
+        <v>7</v>
+      </c>
+      <c r="E16" s="48"/>
+      <c r="F16" s="47">
+        <v>2</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="60"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.6">
+      <c r="B17" s="42"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="47">
+        <v>8</v>
+      </c>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="60"/>
+    </row>
+    <row r="18" spans="2:12" ht="16.2" thickBot="1">
+      <c r="B18" s="42"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="47">
+        <v>9</v>
+      </c>
+      <c r="E18" s="48"/>
+      <c r="F18" s="47">
+        <v>5</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="2:12" ht="16.8" thickTop="1" thickBot="1">
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="27"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
-      <selection activeCell="J3" sqref="J3"/>
+    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
+      <selection activeCell="W13" sqref="W13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5524,8 +5578,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
-      <selection activeCell="W13" sqref="W13"/>
+    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
+      <selection activeCell="J3" sqref="J3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5539,7 +5593,7 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="I8:I9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H10:J14">
+  <conditionalFormatting sqref="H10:J18">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>

</xml_diff>

<commit_message>
addOp, subOp pass normal case
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dai_hoc\LSILogicDesign\FLOATING-POINTING_ALU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\TKVM\FLOATING-POINTING_ALU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046CC6E-B135-48CE-B425-0780E1DE10F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632644F8-248B-46CF-9A65-400B44A8DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="13" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>&lt;Revision history&gt;</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Add a number with its multiplicative inverse value</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>testbench and simulation</t>
   </si>
 </sst>
 </file>
@@ -5183,7 +5189,7 @@
   <dimension ref="B2:AS19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="15"/>
@@ -5399,10 +5405,18 @@
       <c r="G10" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="45"/>
+      <c r="H10" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>37</v>
+      </c>
       <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:45" ht="30">
@@ -5416,10 +5430,18 @@
       <c r="G11" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="45"/>
+      <c r="H11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>37</v>
+      </c>
       <c r="L11" s="59"/>
     </row>
     <row r="12" spans="2:45" ht="30">
@@ -5433,10 +5455,18 @@
       <c r="G12" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="45"/>
+      <c r="H12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>37</v>
+      </c>
       <c r="L12" s="60"/>
     </row>
     <row r="13" spans="2:45" ht="30">

</xml_diff>

<commit_message>
add multiop in checklist
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\TKVM\FLOATING-POINTING_ALU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dai_hoc\LSILogicDesign\FLOATING-POINTING_ALU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632644F8-248B-46CF-9A65-400B44A8DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A82072F-0AD0-4E57-851B-6FD874DC193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="13" r:id="rId1"/>
@@ -57,15 +57,15 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Giang Truong Le. Nguyen - Personal View" guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
+    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
     <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
-    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
-    <customWorkbookView name="Giang Truong Le. Nguyen - Personal View" guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>&lt;Revision history&gt;</t>
   </si>
@@ -145,13 +145,7 @@
     <t>Bound Flasher</t>
   </si>
   <si>
-    <t>addOp check</t>
-  </si>
-  <si>
     <t>Check addition operator between 2 positive parameters</t>
-  </si>
-  <si>
-    <t>addOp check in normal cases</t>
   </si>
   <si>
     <t>Check addition operator between a positive parameter and a negative one</t>
@@ -160,25 +154,52 @@
     <t>Check addition operator between 2 negative parameters</t>
   </si>
   <si>
-    <t>addOp check in overflow cases</t>
-  </si>
-  <si>
-    <t>addOp check in underflow cases</t>
-  </si>
-  <si>
-    <t>addOp check in special cases</t>
-  </si>
-  <si>
     <t>Add a number with zero</t>
   </si>
   <si>
     <t>Add a number with its multiplicative inverse value</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>MultiOp check</t>
   </si>
   <si>
-    <t>testbench and simulation</t>
+    <t>MultiOp check in normal cases</t>
+  </si>
+  <si>
+    <t>AddOp check</t>
+  </si>
+  <si>
+    <t>AddOp check in normal cases</t>
+  </si>
+  <si>
+    <t>AddOp check in overflow cases</t>
+  </si>
+  <si>
+    <t>AddOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>AddOp check in special cases</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between 2 negative parameters</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between a positive parameter and a negative one</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between 2 positive parameters</t>
+  </si>
+  <si>
+    <t>Multiply a number with zero</t>
+  </si>
+  <si>
+    <t>MultiOp check in overflow cases</t>
+  </si>
+  <si>
+    <t>MultiOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>MultiOp check in special cases</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="76">
+  <borders count="83">
     <border>
       <left/>
       <right/>
@@ -2168,6 +2189,95 @@
       </top>
       <bottom style="double">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3582,7 +3692,7 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3724,12 +3834,6 @@
     <xf numFmtId="0" fontId="104" fillId="2" borderId="59" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="104" fillId="51" borderId="73" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -3748,9 +3852,6 @@
     <xf numFmtId="0" fontId="44" fillId="51" borderId="51" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="51" borderId="75" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3834,6 +3935,63 @@
     </xf>
     <xf numFmtId="0" fontId="44" fillId="51" borderId="41" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="52" borderId="76" xfId="457" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="65" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="77" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="78" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="2" borderId="79" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="80" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="81" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="59" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="50" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="82" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="82" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="82" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="80" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="586">
@@ -5014,17 +5172,17 @@
       <c r="D22" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
       <c r="N22" s="38" t="s">
         <v>3</v>
       </c>
@@ -5033,21 +5191,21 @@
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D23" s="65">
+      <c r="D23" s="62">
         <v>45371</v>
       </c>
-      <c r="E23" s="67" t="s">
+      <c r="E23" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="61" t="s">
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="58" t="s">
         <v>16</v>
       </c>
       <c r="O23" s="39" t="s">
@@ -5055,18 +5213,18 @@
       </c>
     </row>
     <row r="24" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D24" s="66"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="58">
+      <c r="D24" s="63"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="55">
         <v>45371</v>
       </c>
     </row>
@@ -5107,17 +5265,17 @@
       <c r="D29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="64" t="s">
+      <c r="E29" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
       <c r="N29" s="37" t="s">
         <v>3</v>
       </c>
@@ -5126,45 +5284,45 @@
       <c r="D30" s="40">
         <v>1</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="70"/>
       <c r="N30" s="41"/>
     </row>
     <row r="31" spans="3:15" ht="15.9" customHeight="1">
       <c r="D31" s="40">
         <v>2</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
       <c r="N31" s="41"/>
     </row>
     <row r="32" spans="3:15" ht="15.9" customHeight="1">
       <c r="D32" s="40">
         <v>3</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
       <c r="N32" s="41"/>
     </row>
   </sheetData>
@@ -5186,10 +5344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:AS19"/>
+  <dimension ref="B2:AS30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="15"/>
@@ -5318,16 +5476,16 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:45" ht="18" thickBot="1">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78" t="s">
+      <c r="C7" s="74"/>
+      <c r="D7" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="26"/>
@@ -5335,271 +5493,432 @@
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="2:45" ht="15.6">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="53" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="53" t="s">
+      <c r="F8" s="52"/>
+      <c r="G8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="82" t="s">
+      <c r="J8" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="82" t="s">
+      <c r="K8" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="71" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:45" ht="16.2" thickBot="1">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="54" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="54" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="75"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="72"/>
     </row>
     <row r="10" spans="2:45" ht="30.6" thickTop="1">
       <c r="B10" s="32">
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="90">
+        <v>1</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="90">
+        <v>1</v>
+      </c>
+      <c r="G10" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="47">
-        <v>1</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="47">
-        <v>1</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="45" t="s">
-        <v>37</v>
-      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:45" ht="30">
       <c r="B11" s="42"/>
       <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="47">
+      <c r="D11" s="90"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="90">
         <v>2</v>
       </c>
-      <c r="G11" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="59"/>
+      <c r="G11" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:45" ht="30">
       <c r="B12" s="42"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="47">
+      <c r="D12" s="90"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="90">
         <v>3</v>
       </c>
-      <c r="G12" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="60"/>
+      <c r="G12" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="2:45" ht="30">
       <c r="B13" s="42"/>
       <c r="C13" s="29"/>
-      <c r="D13" s="47">
+      <c r="D13" s="90">
         <v>2</v>
       </c>
-      <c r="E13" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="47">
+      <c r="E13" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="90">
         <v>1</v>
       </c>
-      <c r="G13" s="55" t="s">
-        <v>27</v>
+      <c r="G13" s="92" t="s">
+        <v>26</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
       <c r="K13" s="45"/>
-      <c r="L13" s="60"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="2:45" ht="30">
       <c r="B14" s="42"/>
       <c r="C14" s="29"/>
-      <c r="D14" s="47">
+      <c r="D14" s="90">
         <v>3</v>
       </c>
-      <c r="E14" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="47">
+      <c r="E14" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="90">
         <v>1</v>
       </c>
-      <c r="G14" s="55" t="s">
-        <v>30</v>
+      <c r="G14" s="92" t="s">
+        <v>28</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
       <c r="K14" s="45"/>
-      <c r="L14" s="60"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="2:45" ht="15.6">
       <c r="B15" s="42"/>
       <c r="C15" s="29"/>
-      <c r="D15" s="47">
+      <c r="D15" s="90">
         <v>4</v>
       </c>
-      <c r="E15" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="47">
+      <c r="E15" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="90">
         <v>1</v>
       </c>
-      <c r="G15" s="55" t="s">
-        <v>34</v>
+      <c r="G15" s="92" t="s">
+        <v>29</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
       <c r="K15" s="45"/>
-      <c r="L15" s="60"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="2:45" ht="15.6">
       <c r="B16" s="42"/>
       <c r="C16" s="29"/>
-      <c r="D16" s="47">
-        <v>7</v>
-      </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="47">
+      <c r="D16" s="93"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="93">
         <v>2</v>
       </c>
-      <c r="G16" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="60"/>
+      <c r="G16" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="83"/>
     </row>
     <row r="17" spans="2:12" ht="15.6">
       <c r="B17" s="42"/>
       <c r="C17" s="29"/>
-      <c r="D17" s="47">
-        <v>8</v>
-      </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="60"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="89"/>
     </row>
-    <row r="18" spans="2:12" ht="16.2" thickBot="1">
-      <c r="B18" s="42"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="47">
-        <v>9</v>
-      </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="47">
-        <v>5</v>
-      </c>
-      <c r="G18" s="55"/>
+    <row r="18" spans="2:12" ht="30">
+      <c r="B18" s="84">
+        <v>2</v>
+      </c>
+      <c r="C18" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="99">
+        <v>1</v>
+      </c>
+      <c r="E18" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="99">
+        <v>1</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>40</v>
+      </c>
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="44"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="87"/>
     </row>
-    <row r="19" spans="2:12" ht="16.8" thickTop="1" thickBot="1">
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="27"/>
+    <row r="19" spans="2:12" ht="30">
+      <c r="B19" s="42"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="90">
+        <v>2</v>
+      </c>
+      <c r="G19" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="57"/>
+    </row>
+    <row r="20" spans="2:12" ht="30">
+      <c r="B20" s="42"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="90">
+        <v>3</v>
+      </c>
+      <c r="G20" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="57"/>
+    </row>
+    <row r="21" spans="2:12" ht="30">
+      <c r="B21" s="42"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="90">
+        <v>2</v>
+      </c>
+      <c r="E21" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="90">
+        <v>1</v>
+      </c>
+      <c r="G21" s="92" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="57"/>
+    </row>
+    <row r="22" spans="2:12" ht="30">
+      <c r="B22" s="42"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="90">
+        <v>3</v>
+      </c>
+      <c r="E22" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="90">
+        <v>1</v>
+      </c>
+      <c r="G22" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="57"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.6">
+      <c r="B23" s="42"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="90">
+        <v>4</v>
+      </c>
+      <c r="E23" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="90">
+        <v>1</v>
+      </c>
+      <c r="G23" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="57"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.6">
+      <c r="B24" s="42"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="57"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.6">
+      <c r="B25" s="42"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="57"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.6">
+      <c r="B26" s="42"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="57"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.6">
+      <c r="B27" s="42"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="57"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.6">
+      <c r="B28" s="42"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="90">
+        <v>8</v>
+      </c>
+      <c r="E28" s="91"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="57"/>
+    </row>
+    <row r="29" spans="2:12" ht="16.2" thickBot="1">
+      <c r="B29" s="42"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="90">
+        <v>9</v>
+      </c>
+      <c r="E29" s="91"/>
+      <c r="F29" s="90">
+        <v>5</v>
+      </c>
+      <c r="G29" s="92"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="2:12" ht="16.8" thickTop="1" thickBot="1">
+      <c r="B30" s="47"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="27"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
-      <selection activeCell="W13" sqref="W13"/>
+    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
+      <selection activeCell="J3" sqref="J3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5608,8 +5927,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
-      <selection activeCell="J3" sqref="J3"/>
+    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
+      <selection activeCell="W13" sqref="W13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5623,7 +5942,7 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="I8:I9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H10:J18">
+  <conditionalFormatting sqref="H10:J29">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>

</xml_diff>

<commit_message>
change checklist, update readme
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\TKVM\FLOATING-POINTING_ALU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502AE29C-B033-4BC6-9A9A-B2A92AC3C81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B845A0-D30B-48DA-A337-6F1C782DA00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="13" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>&lt;Revision history&gt;</t>
   </si>
@@ -139,19 +139,10 @@
     <t>Vũ Huỳnh Tấn Phát</t>
   </si>
   <si>
-    <t>Version 01, 03/20/2024</t>
-  </si>
-  <si>
     <t>Bound Flasher</t>
   </si>
   <si>
-    <t>addOp check</t>
-  </si>
-  <si>
     <t>Check addition operator between 2 positive parameters</t>
-  </si>
-  <si>
-    <t>addOp check in normal cases</t>
   </si>
   <si>
     <t>Check addition operator between a positive parameter and a negative one</t>
@@ -160,37 +151,97 @@
     <t>Check addition operator between 2 negative parameters</t>
   </si>
   <si>
-    <t>addOp check in overflow cases</t>
-  </si>
-  <si>
-    <t>addOp check in underflow cases</t>
-  </si>
-  <si>
-    <t>addOp check in special cases</t>
-  </si>
-  <si>
     <t>Add a number with zero</t>
   </si>
   <si>
     <t>Add a number with its multiplicative inverse value</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>MultiOp check</t>
   </si>
   <si>
-    <t>testbench and simulation</t>
+    <t>MultiOp check in normal cases</t>
   </si>
   <si>
-    <t>subOp check in normal cases</t>
+    <t>AddOp check</t>
   </si>
   <si>
-    <t>subOp check in overflow cases</t>
+    <t>AddOp check in normal cases</t>
   </si>
   <si>
-    <t>subOp check in underflow cases</t>
+    <t>AddOp check in overflow cases</t>
   </si>
   <si>
-    <t>subOp check in special cases</t>
+    <t>AddOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>AddOp check in special cases</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between 2 negative parameters</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between a positive parameter and a negative one</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between 2 positive parameters</t>
+  </si>
+  <si>
+    <t>Multiply a number with zero</t>
+  </si>
+  <si>
+    <t>MultiOp check in overflow cases</t>
+  </si>
+  <si>
+    <t>MultiOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>MultiOp check in special cases</t>
+  </si>
+  <si>
+    <t>Version 01, 12/04/2024</t>
+  </si>
+  <si>
+    <t>Check multiplication operator between 2 negative exponent parameters</t>
+  </si>
+  <si>
+    <t>SubOp check</t>
+  </si>
+  <si>
+    <t>SubOp check in normal cases</t>
+  </si>
+  <si>
+    <t>Check subtraction operator between 2 positive parameters</t>
+  </si>
+  <si>
+    <t>Check subtraction operator between 2 negative parameters</t>
+  </si>
+  <si>
+    <t>Check subtraction operator between a positive parameter and a negative one</t>
+  </si>
+  <si>
+    <t>SubOp check in overflow cases</t>
+  </si>
+  <si>
+    <t>SubOp check in underflow cases</t>
+  </si>
+  <si>
+    <t>SubOp check in special cases</t>
+  </si>
+  <si>
+    <t>Subtract zero from a number</t>
+  </si>
+  <si>
+    <t>Subtract a number from zero</t>
+  </si>
+  <si>
+    <t>Subtracttion operator between same numbers</t>
+  </si>
+  <si>
+    <t>Subtract a negative number from a positive one</t>
+  </si>
+  <si>
+    <t>Subtract a positive number from a negative one</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="76">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -2180,6 +2231,112 @@
       </top>
       <bottom style="double">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3594,7 +3751,7 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3736,12 +3893,6 @@
     <xf numFmtId="0" fontId="104" fillId="2" borderId="59" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="104" fillId="51" borderId="73" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -3760,9 +3911,6 @@
     <xf numFmtId="0" fontId="44" fillId="51" borderId="51" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="51" borderId="75" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3778,6 +3926,63 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="72" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="52" borderId="76" xfId="457" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="77" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="2" borderId="78" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="79" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="80" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="59" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="50" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="63" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="65" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="81" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="81" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="81" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="79" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="82" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="83" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3846,6 +4051,9 @@
     </xf>
     <xf numFmtId="0" fontId="44" fillId="51" borderId="41" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="31" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="586">
@@ -4972,7 +5180,7 @@
   <dimension ref="C3:O32"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9" customHeight="1"/>
@@ -5008,7 +5216,7 @@
     </row>
     <row r="14" spans="4:9" ht="15.9" customHeight="1">
       <c r="I14" s="14" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="4:9" ht="15.9" customHeight="1">
@@ -5026,17 +5234,17 @@
       <c r="D22" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
       <c r="N22" s="38" t="s">
         <v>3</v>
       </c>
@@ -5045,21 +5253,21 @@
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D23" s="65">
-        <v>45371</v>
-      </c>
-      <c r="E23" s="67" t="s">
+      <c r="D23" s="81">
+        <v>45394</v>
+      </c>
+      <c r="E23" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="61" t="s">
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="77" t="s">
         <v>16</v>
       </c>
       <c r="O23" s="39" t="s">
@@ -5067,18 +5275,18 @@
       </c>
     </row>
     <row r="24" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D24" s="66"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="58">
+      <c r="D24" s="82"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="87"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="78"/>
+      <c r="O24" s="55">
         <v>45371</v>
       </c>
     </row>
@@ -5119,17 +5327,17 @@
       <c r="D29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="64" t="s">
+      <c r="E29" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80"/>
       <c r="N29" s="37" t="s">
         <v>3</v>
       </c>
@@ -5138,45 +5346,45 @@
       <c r="D30" s="40">
         <v>1</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
       <c r="N30" s="41"/>
     </row>
     <row r="31" spans="3:15" ht="15.9" customHeight="1">
       <c r="D31" s="40">
         <v>2</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
       <c r="N31" s="41"/>
     </row>
     <row r="32" spans="3:15" ht="15.9" customHeight="1">
       <c r="D32" s="40">
         <v>3</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
       <c r="N32" s="41"/>
     </row>
   </sheetData>
@@ -5198,10 +5406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:AS26"/>
+  <dimension ref="B2:AS34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="15"/>
@@ -5330,16 +5538,16 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:45" ht="18" thickBot="1">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="95"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="26"/>
@@ -5347,413 +5555,525 @@
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="2:45" ht="15.6">
-      <c r="B8" s="52"/>
-      <c r="C8" s="53" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="53" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="53" t="s">
+      <c r="F8" s="52"/>
+      <c r="G8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="80" t="s">
+      <c r="I8" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="82" t="s">
+      <c r="J8" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="82" t="s">
+      <c r="K8" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="90" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:45" ht="16.2" thickBot="1">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="54" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="54" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="75"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="91"/>
     </row>
     <row r="10" spans="2:45" ht="30.6" thickTop="1">
       <c r="B10" s="32">
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="47">
+        <v>32</v>
+      </c>
+      <c r="D10" s="65">
         <v>1</v>
       </c>
-      <c r="E10" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="47">
+      <c r="E10" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="65">
         <v>1</v>
       </c>
-      <c r="G10" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="45" t="s">
-        <v>37</v>
-      </c>
+      <c r="G10" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="44"/>
     </row>
     <row r="11" spans="2:45" ht="30">
       <c r="B11" s="42"/>
       <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="47">
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="65">
         <v>2</v>
       </c>
-      <c r="G11" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="59"/>
+      <c r="G11" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:45" ht="30">
       <c r="B12" s="42"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="47">
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="65">
         <v>3</v>
       </c>
-      <c r="G12" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="60"/>
+      <c r="G12" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="2:45" ht="30">
       <c r="B13" s="42"/>
       <c r="C13" s="29"/>
-      <c r="D13" s="47">
+      <c r="D13" s="65">
         <v>2</v>
       </c>
-      <c r="E13" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="47">
+      <c r="E13" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="65">
         <v>1</v>
       </c>
-      <c r="G13" s="55" t="s">
-        <v>27</v>
+      <c r="G13" s="67" t="s">
+        <v>25</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
       <c r="K13" s="45"/>
-      <c r="L13" s="60"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="2:45" ht="30">
       <c r="B14" s="42"/>
       <c r="C14" s="29"/>
-      <c r="D14" s="47">
+      <c r="D14" s="65">
         <v>3</v>
       </c>
-      <c r="E14" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="47">
+      <c r="E14" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="65">
         <v>1</v>
       </c>
-      <c r="G14" s="55" t="s">
-        <v>30</v>
+      <c r="G14" s="67" t="s">
+        <v>27</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="30"/>
       <c r="K14" s="45"/>
-      <c r="L14" s="60"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="2:45" ht="15.6">
       <c r="B15" s="42"/>
       <c r="C15" s="29"/>
-      <c r="D15" s="47">
+      <c r="D15" s="65">
         <v>4</v>
       </c>
-      <c r="E15" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="47">
+      <c r="E15" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="65">
         <v>1</v>
       </c>
-      <c r="G15" s="55" t="s">
-        <v>34</v>
+      <c r="G15" s="67" t="s">
+        <v>28</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
       <c r="K15" s="45"/>
-      <c r="L15" s="60"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="2:45" ht="15.6">
       <c r="B16" s="42"/>
       <c r="C16" s="29"/>
-      <c r="D16" s="47">
-        <v>7</v>
-      </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="47">
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="68">
         <v>2</v>
       </c>
-      <c r="G16" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="60"/>
+      <c r="G16" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="76"/>
     </row>
-    <row r="17" spans="2:12" ht="30">
+    <row r="17" spans="2:12" ht="15.6">
       <c r="B17" s="42"/>
       <c r="C17" s="29"/>
-      <c r="D17" s="47">
-        <v>8</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="47">
-        <v>1</v>
-      </c>
-      <c r="G17" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="60"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="64"/>
     </row>
     <row r="18" spans="2:12" ht="30">
-      <c r="B18" s="42"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="47">
+      <c r="B18" s="59">
         <v>2</v>
       </c>
-      <c r="G18" s="55" t="s">
+      <c r="C18" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="60"/>
+      <c r="D18" s="74">
+        <v>1</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="74">
+        <v>1</v>
+      </c>
+      <c r="G18" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="62"/>
     </row>
     <row r="19" spans="2:12" ht="30">
       <c r="B19" s="42"/>
       <c r="C19" s="29"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="47">
-        <v>3</v>
-      </c>
-      <c r="G19" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="45" t="s">
+      <c r="D19" s="65"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="65">
+        <v>2</v>
+      </c>
+      <c r="G19" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="60"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="57"/>
     </row>
     <row r="20" spans="2:12" ht="30">
       <c r="B20" s="42"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="47">
-        <v>1</v>
-      </c>
-      <c r="G20" s="55" t="s">
-        <v>27</v>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="65">
+        <v>3</v>
+      </c>
+      <c r="G20" s="67" t="s">
+        <v>38</v>
       </c>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
       <c r="K20" s="45"/>
-      <c r="L20" s="60"/>
+      <c r="L20" s="57"/>
     </row>
     <row r="21" spans="2:12" ht="30">
       <c r="B21" s="42"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="47">
+      <c r="D21" s="65">
+        <v>2</v>
+      </c>
+      <c r="E21" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="65">
         <v>1</v>
       </c>
-      <c r="G21" s="55" t="s">
-        <v>30</v>
+      <c r="G21" s="67" t="s">
+        <v>39</v>
       </c>
       <c r="H21" s="30"/>
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
       <c r="K21" s="45"/>
-      <c r="L21" s="60"/>
+      <c r="L21" s="57"/>
     </row>
-    <row r="22" spans="2:12" ht="15.6">
+    <row r="22" spans="2:12" ht="30">
       <c r="B22" s="42"/>
       <c r="C22" s="29"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="47">
+      <c r="D22" s="65">
+        <v>3</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="65">
         <v>1</v>
       </c>
-      <c r="G22" s="55" t="s">
-        <v>34</v>
+      <c r="G22" s="67" t="s">
+        <v>45</v>
       </c>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
       <c r="J22" s="30"/>
       <c r="K22" s="45"/>
-      <c r="L22" s="60"/>
+      <c r="L22" s="57"/>
     </row>
     <row r="23" spans="2:12" ht="15.6">
       <c r="B23" s="42"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="47">
-        <v>2</v>
-      </c>
-      <c r="G23" s="55" t="s">
-        <v>35</v>
+      <c r="D23" s="65">
+        <v>4</v>
+      </c>
+      <c r="E23" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="65">
+        <v>1</v>
+      </c>
+      <c r="G23" s="67" t="s">
+        <v>40</v>
       </c>
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
       <c r="J23" s="30"/>
       <c r="K23" s="45"/>
-      <c r="L23" s="60"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="2:12" ht="15.6">
       <c r="B24" s="42"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="55"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
       <c r="K24" s="45"/>
-      <c r="L24" s="60"/>
+      <c r="L24" s="57"/>
     </row>
-    <row r="25" spans="2:12" ht="16.2" thickBot="1">
-      <c r="B25" s="42"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="55"/>
+    <row r="25" spans="2:12" ht="30">
+      <c r="B25" s="59">
+        <v>3</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="74">
+        <v>1</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="65">
+        <v>1</v>
+      </c>
+      <c r="G25" s="67" t="s">
+        <v>48</v>
+      </c>
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
       <c r="J25" s="30"/>
       <c r="K25" s="45"/>
-      <c r="L25" s="44"/>
+      <c r="L25" s="57"/>
     </row>
-    <row r="26" spans="2:12" ht="16.8" thickTop="1" thickBot="1">
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="27"/>
+    <row r="26" spans="2:12" ht="30">
+      <c r="B26" s="42"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="65">
+        <v>2</v>
+      </c>
+      <c r="G26" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="57"/>
+    </row>
+    <row r="27" spans="2:12" ht="30">
+      <c r="B27" s="42"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="65">
+        <v>3</v>
+      </c>
+      <c r="G27" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="57"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.6">
+      <c r="B28" s="42"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="100">
+        <v>2</v>
+      </c>
+      <c r="E28" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="65">
+        <v>1</v>
+      </c>
+      <c r="G28" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="57"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.6">
+      <c r="B29" s="42"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="100">
+        <v>3</v>
+      </c>
+      <c r="E29" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="65">
+        <v>1</v>
+      </c>
+      <c r="G29" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="57"/>
+    </row>
+    <row r="30" spans="2:12" ht="15.6">
+      <c r="B30" s="42"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="65">
+        <v>4</v>
+      </c>
+      <c r="E30" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="65">
+        <v>1</v>
+      </c>
+      <c r="G30" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="57"/>
+    </row>
+    <row r="31" spans="2:12" ht="15.6">
+      <c r="B31" s="42"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="68">
+        <v>2</v>
+      </c>
+      <c r="G31" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="57"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.6">
+      <c r="B32" s="42"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="65">
+        <v>3</v>
+      </c>
+      <c r="G32" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="57"/>
+    </row>
+    <row r="33" spans="2:12" ht="16.2" thickBot="1">
+      <c r="B33" s="42"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="44"/>
+    </row>
+    <row r="34" spans="2:12" ht="16.8" thickTop="1" thickBot="1">
+      <c r="B34" s="47"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="27"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -5782,7 +6102,7 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="I8:I9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H10:J25">
+  <conditionalFormatting sqref="H10:J33">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"OK with reason"</formula>
     </cfRule>

</xml_diff>

<commit_message>
testing FP_ALU, update documents
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dai_hoc\LSILogicDesign\FLOATING-POINTING_ALU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B845A0-D30B-48DA-A337-6F1C782DA00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789B73A8-AADA-425A-AE29-1396CE6F8CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="643" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,15 +57,15 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
+    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
     <customWorkbookView name="Giang Truong Le. Nguyen - Personal View" guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="3"/>
-    <customWorkbookView name="Phong Thanh. Phan - Personal View" guid="{BBCD1273-FB62-4046-AADE-F9CEEA687EB3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="5"/>
-    <customWorkbookView name="Hung Quang. Truong - Personal View" guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1864" windowHeight="1218" activeSheetId="6"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>&lt;Revision history&gt;</t>
   </si>
@@ -229,19 +229,16 @@
     <t>SubOp check in special cases</t>
   </si>
   <si>
-    <t>Subtract zero from a number</t>
-  </si>
-  <si>
-    <t>Subtract a number from zero</t>
-  </si>
-  <si>
-    <t>Subtracttion operator between same numbers</t>
-  </si>
-  <si>
     <t>Subtract a negative number from a positive one</t>
   </si>
   <si>
     <t>Subtract a positive number from a negative one</t>
+  </si>
+  <si>
+    <t>Subtract zero from a number, and a number from zero</t>
+  </si>
+  <si>
+    <t>Subtracttion operator between 2 alike numbers</t>
   </si>
 </sst>
 </file>
@@ -3751,7 +3748,7 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3983,6 +3980,9 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="83" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="31" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4052,8 +4052,20 @@
     <xf numFmtId="0" fontId="44" fillId="51" borderId="41" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="2" borderId="31" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="64" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="31" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="2" borderId="13" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="13" xfId="86" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="86" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="586">
@@ -5234,17 +5246,17 @@
       <c r="D22" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="81"/>
       <c r="N22" s="38" t="s">
         <v>3</v>
       </c>
@@ -5253,21 +5265,21 @@
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D23" s="81">
+      <c r="D23" s="82">
         <v>45394</v>
       </c>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="85"/>
-      <c r="N23" s="77" t="s">
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="78" t="s">
         <v>16</v>
       </c>
       <c r="O23" s="39" t="s">
@@ -5275,17 +5287,17 @@
       </c>
     </row>
     <row r="24" spans="3:15" ht="15.9" customHeight="1">
-      <c r="D24" s="82"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="78"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="79"/>
       <c r="O24" s="55">
         <v>45371</v>
       </c>
@@ -5327,17 +5339,17 @@
       <c r="D29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="80"/>
-      <c r="M29" s="80"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
       <c r="N29" s="37" t="s">
         <v>3</v>
       </c>
@@ -5346,45 +5358,45 @@
       <c r="D30" s="40">
         <v>1</v>
       </c>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-      <c r="M30" s="89"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
       <c r="N30" s="41"/>
     </row>
     <row r="31" spans="3:15" ht="15.9" customHeight="1">
       <c r="D31" s="40">
         <v>2</v>
       </c>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="79"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="80"/>
       <c r="N31" s="41"/>
     </row>
     <row r="32" spans="3:15" ht="15.9" customHeight="1">
       <c r="D32" s="40">
         <v>3</v>
       </c>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="79"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
-      <c r="M32" s="79"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
       <c r="N32" s="41"/>
     </row>
   </sheetData>
@@ -5538,14 +5550,14 @@
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:45" ht="18" thickBot="1">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="94" t="s">
+      <c r="C7" s="94"/>
+      <c r="D7" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="96"/>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
       <c r="H7" s="25"/>
@@ -5567,19 +5579,19 @@
       <c r="G8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="96" t="s">
+      <c r="H8" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="96" t="s">
+      <c r="I8" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="98" t="s">
+      <c r="J8" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="98" t="s">
+      <c r="K8" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="90" t="s">
+      <c r="L8" s="91" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5600,11 +5612,11 @@
       <c r="G9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="97"/>
-      <c r="I9" s="97"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="91"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="92"/>
     </row>
     <row r="10" spans="2:45" ht="30.6" thickTop="1">
       <c r="B10" s="32">
@@ -5921,7 +5933,7 @@
     <row r="26" spans="2:12" ht="30">
       <c r="B26" s="42"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="100"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="66"/>
       <c r="F26" s="65">
         <v>2</v>
@@ -5938,7 +5950,7 @@
     <row r="27" spans="2:12" ht="30">
       <c r="B27" s="42"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="100"/>
+      <c r="D27" s="77"/>
       <c r="E27" s="66"/>
       <c r="F27" s="65">
         <v>3</v>
@@ -5955,7 +5967,7 @@
     <row r="28" spans="2:12" ht="15.6">
       <c r="B28" s="42"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="100">
+      <c r="D28" s="77">
         <v>2</v>
       </c>
       <c r="E28" s="66" t="s">
@@ -5965,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="67" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H28" s="30"/>
       <c r="I28" s="30"/>
@@ -5976,7 +5988,7 @@
     <row r="29" spans="2:12" ht="15.6">
       <c r="B29" s="42"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="100">
+      <c r="D29" s="77">
         <v>3</v>
       </c>
       <c r="E29" s="66" t="s">
@@ -5986,7 +5998,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="67" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="30"/>
@@ -5994,7 +6006,7 @@
       <c r="K29" s="45"/>
       <c r="L29" s="57"/>
     </row>
-    <row r="30" spans="2:12" ht="15.6">
+    <row r="30" spans="2:12" ht="30">
       <c r="B30" s="42"/>
       <c r="C30" s="29"/>
       <c r="D30" s="65">
@@ -6003,11 +6015,11 @@
       <c r="E30" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="65">
+      <c r="F30" s="68">
         <v>1</v>
       </c>
-      <c r="G30" s="67" t="s">
-        <v>54</v>
+      <c r="G30" s="70" t="s">
+        <v>56</v>
       </c>
       <c r="H30" s="30"/>
       <c r="I30" s="30"/>
@@ -6019,12 +6031,12 @@
       <c r="B31" s="42"/>
       <c r="C31" s="29"/>
       <c r="D31" s="65"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="68">
+      <c r="E31" s="101"/>
+      <c r="F31" s="103">
         <v>2</v>
       </c>
-      <c r="G31" s="70" t="s">
-        <v>55</v>
+      <c r="G31" s="104" t="s">
+        <v>57</v>
       </c>
       <c r="H31" s="30"/>
       <c r="I31" s="30"/>
@@ -6036,13 +6048,9 @@
       <c r="B32" s="42"/>
       <c r="C32" s="29"/>
       <c r="D32" s="65"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="65">
-        <v>3</v>
-      </c>
-      <c r="G32" s="70" t="s">
-        <v>56</v>
-      </c>
+      <c r="E32" s="101"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
       <c r="H32" s="30"/>
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
@@ -6054,8 +6062,8 @@
       <c r="C33" s="29"/>
       <c r="D33" s="65"/>
       <c r="E33" s="66"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="67"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="102"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
       <c r="J33" s="30"/>
@@ -6077,8 +6085,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
-      <selection activeCell="J3" sqref="J3"/>
+    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
+      <selection activeCell="W13" sqref="W13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -6087,8 +6095,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{C61E42EC-A28A-4F34-B1F0-5B0C369C3BFF}" scale="70">
-      <selection activeCell="W13" sqref="W13"/>
+    <customSheetView guid="{D6408F3F-69A9-4377-B307-B0A0F5ECDF86}">
+      <selection activeCell="J3" sqref="J3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>